<commit_message>
added comments to scanner tests
</commit_message>
<xml_diff>
--- a/Tests/UnitTests/ScannerServiceUnitTests/problem.xlsx
+++ b/Tests/UnitTests/ScannerServiceUnitTests/problem.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\אלינור\Desktop\לימודים\סמסטר ז\פרויקט גמר\OptimusQ\Tests\UnitTests\ScannerServiceUnitTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\rulid\PycharmProjects\RecoSysAviRepo\OptimusQ\Tests\UnitTests\ScannerServiceUnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BBFEE4-7E67-4D74-B37B-A1AD65ED93E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8E388A-6648-4AA2-AF20-AEC8E19C0FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B3AEB19-12A4-494D-AC45-90131E7808F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>url</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>http://do-intl-work-from-home-in-usas-ok.live/?cc=bFPnjiCpmSJE9VjbzRMMAdtik5czzNHHQ4X2nQsAKVj4GYCh9xgV8Zcc54a6dALwWaRFJZGoNjJAYI77gkYTWTvCaXtZaHsImJq86_BsVZ6XW__GAtffiBMML3qyP_ortu7g7S-0VMThBWGm_YObmXtOUxMBNRwIRjdQ_PzPs3GJyGC32GzBImVEwP1rDL8jGPUcq5pvRXUnBN4k1p_YeFWtEaReQ4iL7D-iUnrCPo9vntj71M6HQnoDHTSEhndp07fE-WvGjOoJEgClf1oIMuQMcRBAQo01-Hq1VeoKTWrY6X7TYjmjXUkZN2k2hBT_zKeYNorTWjYqVPYVi7iG86DPZByyyNXFtkdOldU7idmEy1owfBKYk0_5BFOcD8xpS1GTsfxD3ZdTS-cCeH-C29U2L94Os_0DMk0Lh0D30L6EExE5D5K-X6uMTh9MVVhjNbfKeoymzxt4cnWlaHyN03jn9LKRkBn6VThrIvPHiO2wLnJR6TNrIQH1jOUUMTcC-nfk21iKyQeuutprnWyNWO3wNUll-dTwmcrcTR86UHGqvJezWktC-sSud8kg3Z64NKWc2Xl5dXBgs9SZtu4qmyUVH85Nrk_F3J_Ru-FK6I5oTBEK60wg0A2TkDlCWUPIb5g9nugFwzxRoLuKvGhhmSbMeqXc0OIbbJ60nqyYMfvI0PpFNX05yCTOwPnNehmWlINUqwnjTRe3W8xAkwATmWX0dt_Ni_iLPlrAM0iiHMDZQngMgw_a0opqbczA8MsVyAl583ImUNp7XSP_lp08j33_qmpQbZG2gns9Jkwr-39n5zuBa-mA4LA3ESSt_TZPbhWu3wXEPK1QSKm4nXQodPRuIdhk55P-0WTLFYkS8HFHe0eA7KHe910-sg7ryEUATe4eEBXXxZ4XSoUYtDP0EoXXF1Og9Fynt6EI0SZgvMoN_9iGkscHq7_vaw3yt__lUYzSj9nuloWLL7-YzLsoiEo8bluRTkOt27i2RpGfK0-VSFsJ424oVxncZkoAIgLOt0vYrc1q1Rf4wGS2Eg3l-HS0H3FdX2xh3cMOZ5Ua3dDacUp_TndrnQY-mx_9M0BmoTYpMIOSwDu367mU5Afat4SjQmIDEsf84yLEJtJAjbC1Ol5iXPg-QJql4QEROL7COVo4i_8eeu-JH2AiyMHr0vbHzaQnnNM_COe8IxlL76JOklacn5n1ypYs-9Q&amp;tbid=1313561&amp;tbland=view&amp;tbserp=search</t>
-  </si>
-  <si>
-    <t>https://findonlinejobsopen.space/?sub1=10322103&amp;sub2=nationmediagroup-dailynation&amp;sub3=2021-05-15+19%3A19%3A40&amp;adtitle=Getting+an+Online+Job+in+the+USA+May+be+Easier+Than+You+Think&amp;pxtb[id]=1319061&amp;pxtb[ec]=click_event&amp;pxtb[cid]=GiA4LP56dcfXEfkPFYgOpFyNOP_Q2Zeet5iEoO4n9z29iiDl7E8ovLLp1uTzw7qQAQ#tblciGiA4LP56dcfXEfkPFYgOpFyNOP_Q2Zeet5iEoO4n9z29iiDl7E8ovLLp1uTzw7qQAQ</t>
   </si>
   <si>
     <t>https://fetch-miami-real-estate-intl.fyi/?sub_id=taboola_34441_System1_MiamiRE_all_ALL_vinenewz-top10viral&amp;ref=taboola_vinenewz-top10viral#tblciGiB5PUjoGbwJtLlviWkTqJaWioH5rh_OWsYWcsuvFLds0CDhu0c</t>
@@ -302,7 +299,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -348,7 +345,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -644,445 +641,440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A4FBA8-5CEF-4191-9675-FE6FDF71C2D9}">
-  <dimension ref="A1:A86"/>
+  <dimension ref="A1:A85"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.3984375" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add unittests to Scanner Service
</commit_message>
<xml_diff>
--- a/Tests/UnitTests/ScannerServiceUnitTests/problem.xlsx
+++ b/Tests/UnitTests/ScannerServiceUnitTests/problem.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\rulid\PycharmProjects\RecoSysAviRepo\OptimusQ\Tests\UnitTests\ScannerServiceUnitTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\אלינור\Desktop\לימודים\סמסטר ז\פרויקט גמר\OptimusQ\Tests\UnitTests\ScannerServiceUnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8E388A-6648-4AA2-AF20-AEC8E19C0FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AE48E2-77B4-473C-94CB-04EA478B10DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B3AEB19-12A4-494D-AC45-90131E7808F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>url</t>
   </si>
@@ -190,12 +190,6 @@
   </si>
   <si>
     <t>https://smartermoney.mzansireview.co.za/smart_debt_relief?utm_term=8496c3_Do+You+Qualify+For+This+Debt+Relief+Program%3F_https%3A%2F%2Fconsole.brax-cdn.com%2Fcreatives%2Fd636ea4e-c282-433f-a4ba-d3d85f1a13d7%2Fyellow_1000x600_a42bc17f9dc79b4f7d81b5c7e7f0ab15.png&amp;utm_source=taboola&amp;utm_campaign=5681910&amp;utm_medium=disqus-widget-bdnews24en&amp;utm_content=2917461867#tblciGiC1RBXo43We7hwS9FJQjvsQQF-xbe5gmjKCPXQBT5Jx3yCVzUc</t>
-  </si>
-  <si>
-    <t>https://www.businessinsider.com/disney-drive-in-cinema-tickets-melbourne-2021-2021-2?IR=T</t>
-  </si>
-  <si>
-    <t>https://apnews.com/afs:Content:1514120141?utm_source=taboolabackfill&amp;utm_medium=referral&amp;tblci=GiAId4kjQ6dTOp8dg6bJwUI-8OUfgEHnD44_lOK_M8-l9iD46Eco9-Pc4r661Jts</t>
   </si>
   <si>
     <t>http://be-an-intl-modular-kitchen-ok.live/?cc=sHLXqcwXi5vUMHpbkmDJcN5rEskVFxboCcOMdDRhXndM2-5msliO4fz2QZNE5sK5geNfcIP-Eag8tv97HLrHrTCyUmkEdw88diM_20Dw8cnsvyWqt5WggRPawiW7nM2Nu-ytJRf3U12e2G3mtyGwCWKZc0s_Qv3NxglqEduFPwTHUowGC63ot6O-1FbkaJiNqeDsv40b9ud-5SD3zvKhfQEZWFIz4OCPMHXUeo2T3vOHEav7OyWsnP6Fuy3aa1indmhOvaZU6Jqy3rFjMKJDxtKa8GHEdQ0yr52JdLJ8g6HAl6zK-APIP6m2hyUzRTJC4c89zvQZUSRf6u5l17aWU-LwdGcyvKnuhcf8vHUxwOpEcKuzM2x2iu46oTDr5kCftrNstWCEXkZst2WH8sH5LlLILfkmPfaTb6csFUmccKiklJbL2KGG4m1bqNTi1Dg9FkTNkxKfO-v8TU8CdXoaiZ7tsQQAXDZk3hvmbog54JiJgl9AL7WWU2rxg97AvpgMEujp1vZuroc3-iligE4MPL8SUKf_FAlDF5V-Uzf2ejlBmNEozTv5HXGrurCUQzElerG6E8Gm48tvu8PCWWrA5owyabEg94Rp4bnXWUMMH1qdp6I9LPabI7aSoh15rKqS2o4_MfTcoZUfJhTNf0uoV2EqULyJarwo_kdkuY8QrAx5Vl2dNoGS4a_c-HGngZqHPx7RSKHHfTGkB6QxoFbp6sGMe1FkvsQ_H8xMnboBOy6j7RyP5o4KIr0T21a1LGF-KBcLHEaTv-VDBYWGabIL5Zc1hNumotiUY0HQcPZJwjY-oLvzPR1FpG4GJgVi4fJueHzFuazDRxF51r6rLTLFO8urzHIm1ccsXZ0xonAkFKfwWwa2OJarlQK9YIC7k_wDGItq9UursYMplisuizsq_wqtaepBLJzofUfzbcYYpsxJ-lG4r4IlXCHwPRTq7jMSMq6AvZ5Oj8rtSIV6CNjsvilUwNkYwpJC7XCDwvtwA44CWmljbqQT6q46jnDKqehxKemFox_VZaJvQFUcbYQHzO4BaglpvMTomjbJj4oC8Y0q4ge9qiamIkSKfzMwXZrfFoWGJ-6VLz0agsRSjjXFxfyhP29NF5qGnodtiNrXJLA5QYKVXWgbhs1oKMukx3LMXi4F-7JX0MaYC9bnNc05F2QFWZrP6mqslKtO4b_kkXQeFXy3FQS7cwjjY7sqQXPXK043oJVcfX1Sry3zOPlNg3L9uInff1ChGz3TBaItQA0dqtmBB7Fh9RUguc-fdyskjRcS8KQ4iSSsmTC1qxwCFAGhbs_mr_V5ifXn-dAUgFXhBPdv-sodC3x2p8gSpILfnAoGvuTiVrhMR2HVVGDABZDIF0StgHcuPUysbttowfunJkYHYCFGURe8qmdezKyd1VYNEvMaHeoD-0u37PtdgNcaLuN_-y4DmUw9BBClOVsEWxpZkUfU_DhGHlInAVBUiXc-tdFc0RKwFuq4PUGdd1guUViHJHmy_VCdG757xsM6krk-xg</t>
@@ -299,7 +293,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -345,7 +339,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -641,440 +635,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A4FBA8-5CEF-4191-9675-FE6FDF71C2D9}">
-  <dimension ref="A1:A85"/>
+  <dimension ref="A1:A83"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>